<commit_message>
image extractor 3 changed to their new requirement
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -27,19 +27,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>3 x 5000</t>
+    <t>No. of records in file</t>
   </si>
   <si>
-    <t>58 sec</t>
+    <t>Time taken (sec)</t>
+  </si>
+  <si>
+    <t>Program V1.0</t>
+  </si>
+  <si>
+    <t>Program V2.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -47,16 +53,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -64,12 +97,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,23 +438,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5">
+        <v>9.6254860000000008E-3</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3.833557E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4">
+        <v>5.3933534999999998E-2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.3415134E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>1500</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.9253803199999999</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.57043823800000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5100</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7.3081343929999996</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.7953223250000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>15000</v>
+      </c>
+      <c r="B7" s="3">
+        <v>52.826362029999999</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6.1602283929999997</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>